<commit_message>
Added DAU + MAU metrics
</commit_message>
<xml_diff>
--- a/DataAcquisition/Results/Sheets.xlsx
+++ b/DataAcquisition/Results/Sheets.xlsx
@@ -5,15 +5,32 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Step-by-step statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="Preliminary statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="DAU statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="MAU statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="Step-by-step statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="Preliminary statistics" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>DAU</t>
+  </si>
+  <si>
+    <t>01.01.2018</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>MAU</t>
+  </si>
   <si>
     <t>Stage</t>
   </si>
@@ -421,6 +438,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>14831</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>14831</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -429,22 +504,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -672,7 +747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:D114"/>
   <sheetViews>
@@ -682,21 +757,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0">
         <v>13</v>
@@ -710,7 +785,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0">
         <v>34</v>
@@ -724,7 +799,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0">
         <v>23</v>
@@ -738,7 +813,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0">
         <v>16</v>
@@ -752,7 +827,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0">
         <v>9</v>
@@ -766,7 +841,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0">
         <v>14</v>
@@ -780,7 +855,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0">
         <v>15</v>
@@ -794,7 +869,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0">
         <v>12</v>
@@ -808,7 +883,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0">
         <v>11</v>
@@ -822,7 +897,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0">
         <v>18</v>
@@ -836,7 +911,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0">
         <v>18</v>
@@ -850,7 +925,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0">
         <v>21</v>
@@ -864,7 +939,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0">
         <v>10</v>
@@ -878,7 +953,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0">
         <v>9</v>
@@ -892,7 +967,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0">
         <v>7</v>
@@ -906,7 +981,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0">
         <v>11</v>
@@ -920,7 +995,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" s="0">
         <v>23</v>
@@ -934,7 +1009,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0">
         <v>14</v>
@@ -948,7 +1023,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B20" s="0">
         <v>13</v>
@@ -962,7 +1037,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21" s="0">
         <v>15</v>
@@ -976,7 +1051,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22" s="0">
         <v>13</v>
@@ -990,7 +1065,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B23" s="0">
         <v>14</v>
@@ -1004,7 +1079,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B24" s="0">
         <v>12</v>
@@ -1018,7 +1093,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0">
         <v>15</v>
@@ -1032,7 +1107,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0">
         <v>26</v>
@@ -1046,7 +1121,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B27" s="0">
         <v>15</v>
@@ -1060,7 +1135,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B28" s="0">
         <v>12</v>
@@ -1074,7 +1149,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B29" s="0">
         <v>11</v>
@@ -1088,7 +1163,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B30" s="0">
         <v>15</v>
@@ -1102,7 +1177,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B31" s="0">
         <v>15</v>
@@ -1116,7 +1191,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0">
         <v>20</v>
@@ -1130,7 +1205,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0">
         <v>10</v>
@@ -1144,7 +1219,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B34" s="0">
         <v>16</v>
@@ -1158,7 +1233,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0">
         <v>15</v>
@@ -1172,7 +1247,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B36" s="0">
         <v>17</v>
@@ -1186,7 +1261,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B37" s="0">
         <v>12</v>
@@ -1200,7 +1275,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B38" s="0">
         <v>16</v>
@@ -1214,7 +1289,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B39" s="0">
         <v>8</v>
@@ -1228,7 +1303,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B40" s="0">
         <v>15</v>
@@ -1242,7 +1317,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B41" s="0">
         <v>10</v>
@@ -1256,7 +1331,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B42" s="0">
         <v>13</v>
@@ -1270,7 +1345,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B43" s="0">
         <v>13</v>
@@ -1284,7 +1359,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B44" s="0">
         <v>11</v>
@@ -1298,7 +1373,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B45" s="0">
         <v>19</v>
@@ -1312,7 +1387,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B46" s="0">
         <v>14</v>
@@ -1326,7 +1401,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B47" s="0">
         <v>7</v>
@@ -1340,7 +1415,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B48" s="0">
         <v>8</v>
@@ -1354,7 +1429,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B49" s="0">
         <v>19</v>
@@ -1368,7 +1443,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B50" s="0">
         <v>13</v>
@@ -1382,7 +1457,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B51" s="0">
         <v>13</v>
@@ -1396,7 +1471,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B52" s="0">
         <v>14</v>
@@ -1410,7 +1485,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B53" s="0">
         <v>7</v>
@@ -1424,7 +1499,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B54" s="0">
         <v>16</v>
@@ -1438,7 +1513,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B55" s="0">
         <v>16</v>
@@ -1452,7 +1527,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B56" s="0">
         <v>10</v>
@@ -1466,7 +1541,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B57" s="0">
         <v>10</v>
@@ -1480,7 +1555,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B58" s="0">
         <v>9</v>
@@ -1494,7 +1569,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B59" s="0">
         <v>9</v>
@@ -1508,7 +1583,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B60" s="0">
         <v>15</v>
@@ -1522,7 +1597,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B61" s="0">
         <v>14</v>
@@ -1536,7 +1611,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B62" s="0">
         <v>11</v>
@@ -1550,7 +1625,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B63" s="0">
         <v>20</v>
@@ -1564,7 +1639,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B64" s="0">
         <v>19</v>
@@ -1578,7 +1653,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B65" s="0">
         <v>9</v>
@@ -1592,7 +1667,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B66" s="0">
         <v>16</v>
@@ -1606,7 +1681,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B67" s="0">
         <v>16</v>
@@ -1620,7 +1695,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B68" s="0">
         <v>11</v>
@@ -1634,7 +1709,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B69" s="0">
         <v>15</v>
@@ -1648,7 +1723,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B70" s="0">
         <v>16</v>
@@ -1662,7 +1737,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B71" s="0">
         <v>16</v>
@@ -1676,7 +1751,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B72" s="0">
         <v>10</v>
@@ -1690,7 +1765,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B73" s="0">
         <v>10</v>
@@ -1704,7 +1779,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B74" s="0">
         <v>17</v>
@@ -1718,7 +1793,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B75" s="0">
         <v>11</v>
@@ -1732,7 +1807,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B76" s="0">
         <v>12</v>
@@ -1746,7 +1821,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B77" s="0">
         <v>17</v>
@@ -1760,7 +1835,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B78" s="0">
         <v>14</v>
@@ -1774,7 +1849,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B79" s="0">
         <v>12</v>
@@ -1788,7 +1863,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B80" s="0">
         <v>9</v>
@@ -1802,7 +1877,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B81" s="0">
         <v>11</v>
@@ -1816,7 +1891,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B82" s="0">
         <v>19</v>
@@ -1830,7 +1905,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B83" s="0">
         <v>12</v>
@@ -1844,7 +1919,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B84" s="0">
         <v>13</v>
@@ -1858,7 +1933,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B85" s="0">
         <v>16</v>
@@ -1872,7 +1947,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B86" s="0">
         <v>17</v>
@@ -1886,7 +1961,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B87" s="0">
         <v>10</v>
@@ -1900,7 +1975,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B88" s="0">
         <v>9</v>
@@ -1914,7 +1989,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B89" s="0">
         <v>11</v>
@@ -1928,7 +2003,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B90" s="0">
         <v>21</v>
@@ -1942,7 +2017,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B91" s="0">
         <v>6</v>
@@ -1956,7 +2031,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B92" s="0">
         <v>10</v>
@@ -1970,7 +2045,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B93" s="0">
         <v>11</v>
@@ -1984,7 +2059,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B94" s="0">
         <v>7</v>
@@ -1998,7 +2073,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B95" s="0">
         <v>22</v>
@@ -2012,7 +2087,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B96" s="0">
         <v>11</v>
@@ -2026,7 +2101,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B97" s="0">
         <v>12</v>
@@ -2040,7 +2115,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B98" s="0">
         <v>14</v>
@@ -2054,7 +2129,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B99" s="0">
         <v>10</v>
@@ -2068,7 +2143,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B100" s="0">
         <v>16</v>
@@ -2082,7 +2157,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B101" s="0">
         <v>15</v>
@@ -2096,7 +2171,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B102" s="0">
         <v>15</v>
@@ -2110,7 +2185,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B103" s="0">
         <v>18</v>
@@ -2124,7 +2199,7 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B104" s="0">
         <v>9</v>
@@ -2138,7 +2213,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B105" s="0">
         <v>11</v>
@@ -2152,7 +2227,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B106" s="0">
         <v>15</v>
@@ -2166,7 +2241,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B107" s="0">
         <v>19</v>
@@ -2180,7 +2255,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B108" s="0">
         <v>14</v>
@@ -2194,7 +2269,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B109" s="0">
         <v>7</v>
@@ -2208,7 +2283,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B110" s="0">
         <v>19</v>
@@ -2222,7 +2297,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B111" s="0">
         <v>11</v>
@@ -2236,7 +2311,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -2250,7 +2325,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B113" s="0">
         <v>19</v>
@@ -2264,7 +2339,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B114" s="0">
         <v>10</v>

</xml_diff>

<commit_message>
Added Type property to the Event entity (same in DB), and added new users statistics
</commit_message>
<xml_diff>
--- a/DataAcquisition/Results/Sheets.xlsx
+++ b/DataAcquisition/Results/Sheets.xlsx
@@ -5,17 +5,27 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="DAU statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="MAU statistics" sheetId="2" r:id="rId2"/>
-    <sheet name="Step-by-step statistics" sheetId="3" r:id="rId3"/>
-    <sheet name="Preliminary statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="New Users" sheetId="1" r:id="rId1"/>
+    <sheet name="DAU statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="MAU statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="Step-by-step statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="Preliminary statistics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>01.01.2018</t>
+  </si>
   <si>
     <t>Date</t>
   </si>
@@ -23,9 +33,6 @@
     <t>DAU</t>
   </si>
   <si>
-    <t>01.01.2018</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
@@ -101,15 +108,15 @@
     <t>D10</t>
   </si>
   <si>
+    <t>Converter</t>
+  </si>
+  <si>
     <t>Dead Sea Scrolls</t>
   </si>
   <si>
     <t>Butter Bean</t>
   </si>
   <si>
-    <t>Converter</t>
-  </si>
-  <si>
     <t>Edens Soul</t>
   </si>
   <si>
@@ -212,12 +219,12 @@
     <t>White Pony</t>
   </si>
   <si>
+    <t>The Bean</t>
+  </si>
+  <si>
     <t>Best Friend</t>
   </si>
   <si>
-    <t>The Bean</t>
-  </si>
-  <si>
     <t>Anarchist Cookbook</t>
   </si>
   <si>
@@ -290,15 +297,15 @@
     <t>The Book of Belial</t>
   </si>
   <si>
+    <t>Mr. Boom</t>
+  </si>
+  <si>
     <t>Void</t>
   </si>
   <si>
     <t>The Boomerang</t>
   </si>
   <si>
-    <t>Mr. Boom</t>
-  </si>
-  <si>
     <t>Mega Blast</t>
   </si>
   <si>
@@ -317,12 +324,12 @@
     <t>Guppys Head</t>
   </si>
   <si>
+    <t>Razor Blade</t>
+  </si>
+  <si>
     <t>Wooden Nickel</t>
   </si>
   <si>
-    <t>Razor Blade</t>
-  </si>
-  <si>
     <t>Yum Heart</t>
   </si>
   <si>
@@ -377,13 +384,13 @@
     <t>Moms Box</t>
   </si>
   <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
     <t>Sacrificial Altar</t>
   </si>
   <si>
     <t>The Hourglass</t>
-  </si>
-  <si>
-    <t>Black Hole</t>
   </si>
   <si>
     <t>Teleport</t>
@@ -496,6 +503,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>14831</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -504,22 +540,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -747,7 +783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:D114"/>
   <sheetViews>
@@ -757,21 +793,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0">
         <v>13</v>
@@ -785,7 +821,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0">
         <v>34</v>
@@ -799,7 +835,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0">
         <v>23</v>
@@ -813,7 +849,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0">
         <v>16</v>
@@ -827,7 +863,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0">
         <v>9</v>
@@ -841,7 +877,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0">
         <v>14</v>
@@ -855,7 +891,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0">
         <v>15</v>
@@ -869,7 +905,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0">
         <v>12</v>
@@ -883,7 +919,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0">
         <v>11</v>
@@ -897,7 +933,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0">
         <v>18</v>
@@ -911,7 +947,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0">
         <v>18</v>
@@ -925,7 +961,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0">
         <v>21</v>
@@ -939,7 +975,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0">
         <v>10</v>
@@ -953,7 +989,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0">
         <v>9</v>
@@ -967,7 +1003,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0">
         <v>7</v>
@@ -981,13 +1017,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0">
-        <v>5940</v>
+        <v>9800</v>
       </c>
       <c r="D17" s="0">
         <v>0</v>
@@ -995,13 +1031,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C18" s="0">
-        <v>1380</v>
+        <v>5940</v>
       </c>
       <c r="D18" s="0">
         <v>0</v>
@@ -1009,13 +1045,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0">
-        <v>9800</v>
+        <v>1380</v>
       </c>
       <c r="D19" s="0">
         <v>0</v>
@@ -1023,7 +1059,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0">
         <v>13</v>
@@ -1037,7 +1073,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B21" s="0">
         <v>15</v>
@@ -1051,7 +1087,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="0">
         <v>13</v>
@@ -1065,7 +1101,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0">
         <v>14</v>
@@ -1079,7 +1115,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="0">
         <v>12</v>
@@ -1093,7 +1129,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" s="0">
         <v>15</v>
@@ -1107,7 +1143,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="0">
         <v>26</v>
@@ -1121,7 +1157,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B27" s="0">
         <v>15</v>
@@ -1135,7 +1171,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" s="0">
         <v>12</v>
@@ -1149,7 +1185,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="0">
         <v>11</v>
@@ -1163,7 +1199,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="0">
         <v>15</v>
@@ -1177,7 +1213,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" s="0">
         <v>15</v>
@@ -1191,7 +1227,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B32" s="0">
         <v>20</v>
@@ -1205,7 +1241,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0">
         <v>10</v>
@@ -1219,7 +1255,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0">
         <v>16</v>
@@ -1233,7 +1269,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B35" s="0">
         <v>15</v>
@@ -1247,7 +1283,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B36" s="0">
         <v>17</v>
@@ -1261,7 +1297,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B37" s="0">
         <v>12</v>
@@ -1275,7 +1311,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0">
         <v>16</v>
@@ -1289,7 +1325,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0">
         <v>8</v>
@@ -1303,7 +1339,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B40" s="0">
         <v>15</v>
@@ -1317,7 +1353,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B41" s="0">
         <v>10</v>
@@ -1331,7 +1367,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="0">
         <v>13</v>
@@ -1345,7 +1381,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B43" s="0">
         <v>13</v>
@@ -1359,7 +1395,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B44" s="0">
         <v>11</v>
@@ -1373,7 +1409,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" s="0">
         <v>19</v>
@@ -1387,7 +1423,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B46" s="0">
         <v>14</v>
@@ -1401,7 +1437,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B47" s="0">
         <v>7</v>
@@ -1415,7 +1451,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B48" s="0">
         <v>8</v>
@@ -1429,7 +1465,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B49" s="0">
         <v>19</v>
@@ -1443,7 +1479,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B50" s="0">
         <v>13</v>
@@ -1457,7 +1493,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B51" s="0">
         <v>13</v>
@@ -1471,7 +1507,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B52" s="0">
         <v>14</v>
@@ -1485,7 +1521,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B53" s="0">
         <v>7</v>
@@ -1499,13 +1535,13 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" s="0">
         <v>16</v>
       </c>
       <c r="C54" s="0">
-        <v>10400</v>
+        <v>1600</v>
       </c>
       <c r="D54" s="0">
         <v>0</v>
@@ -1513,13 +1549,13 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B55" s="0">
         <v>16</v>
       </c>
       <c r="C55" s="0">
-        <v>1600</v>
+        <v>10400</v>
       </c>
       <c r="D55" s="0">
         <v>0</v>
@@ -1527,7 +1563,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B56" s="0">
         <v>10</v>
@@ -1541,7 +1577,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B57" s="0">
         <v>10</v>
@@ -1555,7 +1591,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B58" s="0">
         <v>9</v>
@@ -1569,7 +1605,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B59" s="0">
         <v>9</v>
@@ -1583,7 +1619,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B60" s="0">
         <v>15</v>
@@ -1597,7 +1633,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B61" s="0">
         <v>14</v>
@@ -1611,7 +1647,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B62" s="0">
         <v>11</v>
@@ -1625,7 +1661,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B63" s="0">
         <v>20</v>
@@ -1639,7 +1675,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B64" s="0">
         <v>19</v>
@@ -1653,7 +1689,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B65" s="0">
         <v>9</v>
@@ -1667,7 +1703,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B66" s="0">
         <v>16</v>
@@ -1681,7 +1717,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B67" s="0">
         <v>16</v>
@@ -1695,7 +1731,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B68" s="0">
         <v>11</v>
@@ -1709,7 +1745,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B69" s="0">
         <v>15</v>
@@ -1723,7 +1759,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B70" s="0">
         <v>16</v>
@@ -1737,7 +1773,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B71" s="0">
         <v>16</v>
@@ -1751,7 +1787,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B72" s="0">
         <v>10</v>
@@ -1765,7 +1801,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B73" s="0">
         <v>10</v>
@@ -1779,7 +1815,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B74" s="0">
         <v>17</v>
@@ -1793,7 +1829,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B75" s="0">
         <v>11</v>
@@ -1807,7 +1843,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B76" s="0">
         <v>12</v>
@@ -1821,7 +1857,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B77" s="0">
         <v>17</v>
@@ -1835,7 +1871,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B78" s="0">
         <v>14</v>
@@ -1849,7 +1885,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B79" s="0">
         <v>12</v>
@@ -1863,13 +1899,13 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B80" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C80" s="0">
-        <v>5040</v>
+        <v>9310</v>
       </c>
       <c r="D80" s="0">
         <v>0</v>
@@ -1877,13 +1913,13 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B81" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C81" s="0">
-        <v>7480</v>
+        <v>5040</v>
       </c>
       <c r="D81" s="0">
         <v>0</v>
@@ -1891,13 +1927,13 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B82" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C82" s="0">
-        <v>9310</v>
+        <v>7480</v>
       </c>
       <c r="D82" s="0">
         <v>0</v>
@@ -1905,7 +1941,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B83" s="0">
         <v>12</v>
@@ -1919,7 +1955,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B84" s="0">
         <v>13</v>
@@ -1933,7 +1969,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B85" s="0">
         <v>16</v>
@@ -1947,7 +1983,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B86" s="0">
         <v>17</v>
@@ -1961,7 +1997,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B87" s="0">
         <v>10</v>
@@ -1975,7 +2011,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B88" s="0">
         <v>9</v>
@@ -1989,13 +2025,13 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B89" s="0">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C89" s="0">
-        <v>1210</v>
+        <v>3570</v>
       </c>
       <c r="D89" s="0">
         <v>0</v>
@@ -2003,13 +2039,13 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B90" s="0">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C90" s="0">
-        <v>3570</v>
+        <v>1210</v>
       </c>
       <c r="D90" s="0">
         <v>0</v>
@@ -2017,7 +2053,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B91" s="0">
         <v>6</v>
@@ -2031,7 +2067,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B92" s="0">
         <v>10</v>
@@ -2045,7 +2081,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B93" s="0">
         <v>11</v>
@@ -2059,7 +2095,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B94" s="0">
         <v>7</v>
@@ -2073,7 +2109,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B95" s="0">
         <v>22</v>
@@ -2087,7 +2123,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B96" s="0">
         <v>11</v>
@@ -2101,7 +2137,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B97" s="0">
         <v>12</v>
@@ -2115,7 +2151,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B98" s="0">
         <v>14</v>
@@ -2129,7 +2165,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B99" s="0">
         <v>10</v>
@@ -2143,7 +2179,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B100" s="0">
         <v>16</v>
@@ -2157,7 +2193,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B101" s="0">
         <v>15</v>
@@ -2171,7 +2207,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B102" s="0">
         <v>15</v>
@@ -2185,7 +2221,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B103" s="0">
         <v>18</v>
@@ -2199,7 +2235,7 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B104" s="0">
         <v>9</v>
@@ -2213,7 +2249,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B105" s="0">
         <v>11</v>
@@ -2227,7 +2263,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B106" s="0">
         <v>15</v>
@@ -2241,7 +2277,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B107" s="0">
         <v>19</v>
@@ -2255,7 +2291,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B108" s="0">
         <v>14</v>
@@ -2269,13 +2305,13 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B109" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C109" s="0">
-        <v>4200</v>
+        <v>5610</v>
       </c>
       <c r="D109" s="0">
         <v>0</v>
@@ -2283,13 +2319,13 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B110" s="0">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C110" s="0">
-        <v>1520</v>
+        <v>4200</v>
       </c>
       <c r="D110" s="0">
         <v>0</v>
@@ -2297,13 +2333,13 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B111" s="0">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C111" s="0">
-        <v>5610</v>
+        <v>1520</v>
       </c>
       <c r="D111" s="0">
         <v>0</v>
@@ -2311,7 +2347,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -2325,7 +2361,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B113" s="0">
         <v>19</v>
@@ -2339,7 +2375,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B114" s="0">
         <v>10</v>

</xml_diff>

<commit_message>
Added money related statistics
</commit_message>
<xml_diff>
--- a/DataAcquisition/Results/Sheets.xlsx
+++ b/DataAcquisition/Results/Sheets.xlsx
@@ -8,15 +8,17 @@
     <sheet name="New Users" sheetId="1" r:id="rId1"/>
     <sheet name="DAU statistics" sheetId="2" r:id="rId2"/>
     <sheet name="MAU statistics" sheetId="3" r:id="rId3"/>
-    <sheet name="Step-by-step statistics" sheetId="4" r:id="rId4"/>
-    <sheet name="Preliminary statistics" sheetId="5" r:id="rId5"/>
+    <sheet name="Revenue statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="Currency rate" sheetId="5" r:id="rId5"/>
+    <sheet name="Step-by-step statistics" sheetId="6" r:id="rId6"/>
+    <sheet name="Preliminary statistics" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Day</t>
   </si>
@@ -37,6 +39,12 @@
   </si>
   <si>
     <t>MAU</t>
+  </si>
+  <si>
+    <t>Revenue, $</t>
+  </si>
+  <si>
+    <t>Rate, $ / curr</t>
   </si>
   <si>
     <t>Stage</t>
@@ -532,6 +540,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>11054</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.08668104293275829</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -540,22 +606,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -783,7 +849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:D114"/>
   <sheetViews>
@@ -793,21 +859,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0">
         <v>13</v>
@@ -821,7 +887,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0">
         <v>34</v>
@@ -835,7 +901,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0">
         <v>23</v>
@@ -849,7 +915,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0">
         <v>16</v>
@@ -863,7 +929,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0">
         <v>9</v>
@@ -877,7 +943,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0">
         <v>14</v>
@@ -891,7 +957,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0">
         <v>15</v>
@@ -905,7 +971,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0">
         <v>12</v>
@@ -919,7 +985,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0">
         <v>11</v>
@@ -933,7 +999,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0">
         <v>18</v>
@@ -947,7 +1013,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0">
         <v>18</v>
@@ -961,7 +1027,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0">
         <v>21</v>
@@ -975,7 +1041,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0">
         <v>10</v>
@@ -989,7 +1055,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0">
         <v>9</v>
@@ -1003,7 +1069,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0">
         <v>7</v>
@@ -1017,7 +1083,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0">
         <v>14</v>
@@ -1031,7 +1097,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0">
         <v>11</v>
@@ -1045,7 +1111,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0">
         <v>23</v>
@@ -1059,7 +1125,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0">
         <v>13</v>
@@ -1073,7 +1139,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0">
         <v>15</v>
@@ -1087,7 +1153,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0">
         <v>13</v>
@@ -1101,7 +1167,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0">
         <v>14</v>
@@ -1115,7 +1181,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0">
         <v>12</v>
@@ -1129,7 +1195,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0">
         <v>15</v>
@@ -1143,7 +1209,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0">
         <v>26</v>
@@ -1157,7 +1223,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0">
         <v>15</v>
@@ -1171,7 +1237,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0">
         <v>12</v>
@@ -1185,7 +1251,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0">
         <v>11</v>
@@ -1199,7 +1265,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0">
         <v>15</v>
@@ -1213,7 +1279,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0">
         <v>15</v>
@@ -1227,7 +1293,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B32" s="0">
         <v>20</v>
@@ -1241,7 +1307,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" s="0">
         <v>10</v>
@@ -1255,7 +1321,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B34" s="0">
         <v>16</v>
@@ -1269,7 +1335,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0">
         <v>15</v>
@@ -1283,7 +1349,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0">
         <v>17</v>
@@ -1297,7 +1363,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B37" s="0">
         <v>12</v>
@@ -1311,7 +1377,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B38" s="0">
         <v>16</v>
@@ -1325,7 +1391,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0">
         <v>8</v>
@@ -1339,7 +1405,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B40" s="0">
         <v>15</v>
@@ -1353,7 +1419,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B41" s="0">
         <v>10</v>
@@ -1367,7 +1433,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B42" s="0">
         <v>13</v>
@@ -1381,7 +1447,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B43" s="0">
         <v>13</v>
@@ -1395,7 +1461,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B44" s="0">
         <v>11</v>
@@ -1409,7 +1475,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B45" s="0">
         <v>19</v>
@@ -1423,7 +1489,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B46" s="0">
         <v>14</v>
@@ -1437,7 +1503,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B47" s="0">
         <v>7</v>
@@ -1451,7 +1517,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B48" s="0">
         <v>8</v>
@@ -1465,7 +1531,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B49" s="0">
         <v>19</v>
@@ -1479,7 +1545,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B50" s="0">
         <v>13</v>
@@ -1493,7 +1559,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B51" s="0">
         <v>13</v>
@@ -1507,7 +1573,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B52" s="0">
         <v>14</v>
@@ -1521,7 +1587,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B53" s="0">
         <v>7</v>
@@ -1535,7 +1601,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B54" s="0">
         <v>16</v>
@@ -1549,7 +1615,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0">
         <v>16</v>
@@ -1563,7 +1629,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B56" s="0">
         <v>10</v>
@@ -1577,7 +1643,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B57" s="0">
         <v>10</v>
@@ -1591,7 +1657,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0">
         <v>9</v>
@@ -1605,7 +1671,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B59" s="0">
         <v>9</v>
@@ -1619,7 +1685,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B60" s="0">
         <v>15</v>
@@ -1633,7 +1699,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B61" s="0">
         <v>14</v>
@@ -1647,7 +1713,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B62" s="0">
         <v>11</v>
@@ -1661,7 +1727,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B63" s="0">
         <v>20</v>
@@ -1675,7 +1741,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B64" s="0">
         <v>19</v>
@@ -1689,7 +1755,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B65" s="0">
         <v>9</v>
@@ -1703,7 +1769,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B66" s="0">
         <v>16</v>
@@ -1717,7 +1783,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B67" s="0">
         <v>16</v>
@@ -1731,7 +1797,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0">
         <v>11</v>
@@ -1745,7 +1811,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B69" s="0">
         <v>15</v>
@@ -1759,7 +1825,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B70" s="0">
         <v>16</v>
@@ -1773,7 +1839,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B71" s="0">
         <v>16</v>
@@ -1787,7 +1853,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B72" s="0">
         <v>10</v>
@@ -1801,7 +1867,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0">
         <v>10</v>
@@ -1815,7 +1881,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B74" s="0">
         <v>17</v>
@@ -1829,7 +1895,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B75" s="0">
         <v>11</v>
@@ -1843,7 +1909,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B76" s="0">
         <v>12</v>
@@ -1857,7 +1923,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B77" s="0">
         <v>17</v>
@@ -1871,7 +1937,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B78" s="0">
         <v>14</v>
@@ -1885,7 +1951,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B79" s="0">
         <v>12</v>
@@ -1899,7 +1965,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B80" s="0">
         <v>19</v>
@@ -1913,7 +1979,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B81" s="0">
         <v>9</v>
@@ -1927,7 +1993,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B82" s="0">
         <v>11</v>
@@ -1941,7 +2007,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B83" s="0">
         <v>12</v>
@@ -1955,7 +2021,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0">
         <v>13</v>
@@ -1969,7 +2035,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B85" s="0">
         <v>16</v>
@@ -1983,7 +2049,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B86" s="0">
         <v>17</v>
@@ -1997,7 +2063,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B87" s="0">
         <v>10</v>
@@ -2011,7 +2077,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B88" s="0">
         <v>9</v>
@@ -2025,7 +2091,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B89" s="0">
         <v>21</v>
@@ -2039,7 +2105,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B90" s="0">
         <v>11</v>
@@ -2053,7 +2119,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B91" s="0">
         <v>6</v>
@@ -2067,7 +2133,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B92" s="0">
         <v>10</v>
@@ -2081,7 +2147,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B93" s="0">
         <v>11</v>
@@ -2095,7 +2161,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B94" s="0">
         <v>7</v>
@@ -2109,7 +2175,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B95" s="0">
         <v>22</v>
@@ -2123,7 +2189,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B96" s="0">
         <v>11</v>
@@ -2137,7 +2203,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B97" s="0">
         <v>12</v>
@@ -2151,7 +2217,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B98" s="0">
         <v>14</v>
@@ -2165,7 +2231,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B99" s="0">
         <v>10</v>
@@ -2179,7 +2245,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B100" s="0">
         <v>16</v>
@@ -2193,7 +2259,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B101" s="0">
         <v>15</v>
@@ -2207,7 +2273,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B102" s="0">
         <v>15</v>
@@ -2221,7 +2287,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B103" s="0">
         <v>18</v>
@@ -2235,7 +2301,7 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B104" s="0">
         <v>9</v>
@@ -2249,7 +2315,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B105" s="0">
         <v>11</v>
@@ -2263,7 +2329,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B106" s="0">
         <v>15</v>
@@ -2277,7 +2343,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B107" s="0">
         <v>19</v>
@@ -2291,7 +2357,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B108" s="0">
         <v>14</v>
@@ -2305,7 +2371,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B109" s="0">
         <v>11</v>
@@ -2319,7 +2385,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B110" s="0">
         <v>7</v>
@@ -2333,7 +2399,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B111" s="0">
         <v>19</v>
@@ -2347,7 +2413,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B112" s="0">
         <v>20</v>
@@ -2361,7 +2427,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B113" s="0">
         <v>19</v>
@@ -2375,7 +2441,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B114" s="0">
         <v>10</v>

</xml_diff>

<commit_message>
Fixes due to query timeout, and date format in result file
</commit_message>
<xml_diff>
--- a/DataAcquisition/Results/Sheets.xlsx
+++ b/DataAcquisition/Results/Sheets.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>Day</t>
   </si>
@@ -26,9 +26,30 @@
     <t>Users</t>
   </si>
   <si>
+    <t>07.01.2018</t>
+  </si>
+  <si>
+    <t>08.01.2018</t>
+  </si>
+  <si>
     <t>01.01.2018</t>
   </si>
   <si>
+    <t>02.01.2018</t>
+  </si>
+  <si>
+    <t>06.01.2018</t>
+  </si>
+  <si>
+    <t>05.01.2018</t>
+  </si>
+  <si>
+    <t>04.01.2018</t>
+  </si>
+  <si>
+    <t>03.01.2018</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -71,343 +92,343 @@
     <t>Item amount</t>
   </si>
   <si>
+    <t>We Need to Go Deeper!</t>
+  </si>
+  <si>
+    <t>Moms Box</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>Converter</t>
+  </si>
+  <si>
+    <t>Dataminer</t>
+  </si>
+  <si>
+    <t>Mine Crafter</t>
+  </si>
+  <si>
+    <t>Ventricle Razor</t>
+  </si>
+  <si>
+    <t>Crooked Penny</t>
+  </si>
+  <si>
+    <t>Best Friend</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Guppys Head</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>Jar of Flies</t>
+  </si>
+  <si>
+    <t>White Pony</t>
+  </si>
+  <si>
+    <t>Clicker</t>
+  </si>
+  <si>
+    <t>Sprinkler</t>
+  </si>
+  <si>
+    <t>The Jar</t>
+  </si>
+  <si>
+    <t>Book of Shadows</t>
+  </si>
+  <si>
+    <t>Monster Manual</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>Mama Mega!</t>
+  </si>
+  <si>
     <t>Diplopia</t>
   </si>
   <si>
+    <t>The Book of Sin</t>
+  </si>
+  <si>
+    <t>Crystal Ball</t>
+  </si>
+  <si>
+    <t>Remote Detonator</t>
+  </si>
+  <si>
+    <t>Delirious</t>
+  </si>
+  <si>
+    <t>Friendly Ball</t>
+  </si>
+  <si>
+    <t>The Necronomicon</t>
+  </si>
+  <si>
+    <t>Prayer Card</t>
+  </si>
+  <si>
+    <t>Mr. ME!</t>
+  </si>
+  <si>
+    <t>Kamikaze!</t>
+  </si>
+  <si>
+    <t>Unicorn Stump</t>
+  </si>
+  <si>
+    <t>Pandoras Box</t>
+  </si>
+  <si>
+    <t>Glowing Hour Glass</t>
+  </si>
+  <si>
+    <t>Yum Heart</t>
+  </si>
+  <si>
+    <t>Breath of Life</t>
+  </si>
+  <si>
+    <t>Box of Spiders</t>
+  </si>
+  <si>
+    <t>Head of Krampus</t>
+  </si>
+  <si>
+    <t>Shoop Da Whoop!</t>
+  </si>
+  <si>
+    <t>Wooden Nickel</t>
+  </si>
+  <si>
+    <t>The Nail</t>
+  </si>
+  <si>
+    <t>Tear Detonator</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>My Little Unicorn</t>
+  </si>
+  <si>
+    <t>Dads Key</t>
+  </si>
+  <si>
+    <t>The Candle</t>
+  </si>
+  <si>
+    <t>Plan C</t>
+  </si>
+  <si>
+    <t>Magic Fingers</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Forget Me Now</t>
+  </si>
+  <si>
+    <t>Anarchist Cookbook</t>
+  </si>
+  <si>
+    <t>The Boomerang</t>
+  </si>
+  <si>
     <t>Flush!</t>
   </si>
   <si>
-    <t>Prayer Card</t>
+    <t>Glass Cannon</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>The D6</t>
+  </si>
+  <si>
+    <t>Sharp Straw</t>
+  </si>
+  <si>
+    <t>Teleport 2.0</t>
+  </si>
+  <si>
+    <t>Moving Box</t>
+  </si>
+  <si>
+    <t>Void</t>
+  </si>
+  <si>
+    <t>Book of the Dead</t>
+  </si>
+  <si>
+    <t>Blank Card</t>
+  </si>
+  <si>
+    <t>Telekinesis</t>
+  </si>
+  <si>
+    <t>Blood Rights</t>
+  </si>
+  <si>
+    <t>Sacrificial Altar</t>
+  </si>
+  <si>
+    <t>Broken Shovel</t>
+  </si>
+  <si>
+    <t>Crack the Sky</t>
+  </si>
+  <si>
+    <t>Monstros Tooth</t>
+  </si>
+  <si>
+    <t>Razor Blade</t>
+  </si>
+  <si>
+    <t>Compost</t>
+  </si>
+  <si>
+    <t>Metronome</t>
+  </si>
+  <si>
+    <t>Mega Bean</t>
+  </si>
+  <si>
+    <t>The Pinking Shears</t>
+  </si>
+  <si>
+    <t>Dead Sea Scrolls</t>
+  </si>
+  <si>
+    <t>Telepathy for Dummies</t>
+  </si>
+  <si>
+    <t>The Gamekid</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Mr. Boom</t>
+  </si>
+  <si>
+    <t>Edens Soul</t>
+  </si>
+  <si>
+    <t>Brown Nugget</t>
+  </si>
+  <si>
+    <t>Kidney Bean</t>
+  </si>
+  <si>
+    <t>Mystery Gift</t>
+  </si>
+  <si>
+    <t>A Pony</t>
+  </si>
+  <si>
+    <t>Doctors Remote</t>
+  </si>
+  <si>
+    <t>Wait What?</t>
+  </si>
+  <si>
+    <t>Moms Shovel</t>
+  </si>
+  <si>
+    <t>The Book of Belial</t>
+  </si>
+  <si>
+    <t>IV Bag</t>
+  </si>
+  <si>
+    <t>Portable Slot</t>
+  </si>
+  <si>
+    <t>Guppys Paw</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Mega Blast</t>
+  </si>
+  <si>
+    <t>Lemon Mishap</t>
+  </si>
+  <si>
+    <t>How to Jump</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>The Hourglass</t>
+  </si>
+  <si>
+    <t>Notched Axe</t>
+  </si>
+  <si>
+    <t>Potato Peeler</t>
+  </si>
+  <si>
+    <t>Box of Friends</t>
+  </si>
+  <si>
+    <t>The Bean</t>
+  </si>
+  <si>
+    <t>Tammys Head</t>
+  </si>
+  <si>
+    <t>Dull Razor</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>D100</t>
+  </si>
+  <si>
+    <t>D Infinity</t>
+  </si>
+  <si>
+    <t>Book of Secrets</t>
   </si>
   <si>
     <t>Book of Revelations</t>
   </si>
   <si>
-    <t>Guppys Paw</t>
-  </si>
-  <si>
-    <t>Metronome</t>
-  </si>
-  <si>
-    <t>Head of Krampus</t>
-  </si>
-  <si>
-    <t>Mr. ME!</t>
-  </si>
-  <si>
-    <t>The Nail</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>Shoop Da Whoop!</t>
-  </si>
-  <si>
-    <t>Glass Cannon</t>
-  </si>
-  <si>
-    <t>Book of Secrets</t>
-  </si>
-  <si>
-    <t>We Need to Go Deeper!</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>Converter</t>
-  </si>
-  <si>
-    <t>Dead Sea Scrolls</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Deck of Cards</t>
   </si>
   <si>
     <t>Butter Bean</t>
   </si>
   <si>
-    <t>Edens Soul</t>
-  </si>
-  <si>
-    <t>Moving Box</t>
-  </si>
-  <si>
-    <t>Potato Peeler</t>
-  </si>
-  <si>
-    <t>Plan C</t>
-  </si>
-  <si>
-    <t>Remote Detonator</t>
-  </si>
-  <si>
-    <t>The Candle</t>
-  </si>
-  <si>
-    <t>Crack the Sky</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>Crystal Ball</t>
-  </si>
-  <si>
-    <t>Telekinesis</t>
-  </si>
-  <si>
-    <t>Teleport 2.0</t>
-  </si>
-  <si>
-    <t>Monstros Tooth</t>
-  </si>
-  <si>
-    <t>Kidney Bean</t>
-  </si>
-  <si>
-    <t>Tammys Head</t>
-  </si>
-  <si>
-    <t>Deck of Cards</t>
-  </si>
-  <si>
-    <t>Glowing Hour Glass</t>
-  </si>
-  <si>
-    <t>Brown Nugget</t>
-  </si>
-  <si>
-    <t>Broken Shovel</t>
-  </si>
-  <si>
-    <t>D Infinity</t>
-  </si>
-  <si>
-    <t>D20</t>
-  </si>
-  <si>
-    <t>Doctors Remote</t>
-  </si>
-  <si>
-    <t>Lemon Mishap</t>
-  </si>
-  <si>
-    <t>Breath of Life</t>
-  </si>
-  <si>
-    <t>Scissors</t>
-  </si>
-  <si>
-    <t>Pandoras Box</t>
-  </si>
-  <si>
-    <t>Placebo</t>
-  </si>
-  <si>
-    <t>Moms Shovel</t>
-  </si>
-  <si>
-    <t>Crooked Penny</t>
-  </si>
-  <si>
-    <t>Mine Crafter</t>
-  </si>
-  <si>
-    <t>Friendly Ball</t>
-  </si>
-  <si>
     <t>Moms Bottle of Pills</t>
-  </si>
-  <si>
-    <t>Dads Key</t>
-  </si>
-  <si>
-    <t>White Pony</t>
-  </si>
-  <si>
-    <t>The Bean</t>
-  </si>
-  <si>
-    <t>Best Friend</t>
-  </si>
-  <si>
-    <t>Anarchist Cookbook</t>
-  </si>
-  <si>
-    <t>Delirious</t>
-  </si>
-  <si>
-    <t>IV Bag</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>The Gamekid</t>
-  </si>
-  <si>
-    <t>Box of Spiders</t>
-  </si>
-  <si>
-    <t>Clicker</t>
-  </si>
-  <si>
-    <t>Blank Card</t>
-  </si>
-  <si>
-    <t>Mama Mega!</t>
-  </si>
-  <si>
-    <t>My Little Unicorn</t>
-  </si>
-  <si>
-    <t>Coupon</t>
-  </si>
-  <si>
-    <t>Dataminer</t>
-  </si>
-  <si>
-    <t>Sprinkler</t>
-  </si>
-  <si>
-    <t>The Pinking Shears</t>
-  </si>
-  <si>
-    <t>Undefined</t>
-  </si>
-  <si>
-    <t>Telepathy for Dummies</t>
-  </si>
-  <si>
-    <t>D100</t>
-  </si>
-  <si>
-    <t>Tear Detonator</t>
-  </si>
-  <si>
-    <t>Blood Rights</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>Dull Razor</t>
-  </si>
-  <si>
-    <t>Jar of Flies</t>
-  </si>
-  <si>
-    <t>Wait What?</t>
-  </si>
-  <si>
-    <t>The Book of Belial</t>
-  </si>
-  <si>
-    <t>Mr. Boom</t>
-  </si>
-  <si>
-    <t>Void</t>
-  </si>
-  <si>
-    <t>The Boomerang</t>
-  </si>
-  <si>
-    <t>Mega Blast</t>
-  </si>
-  <si>
-    <t>Book of Shadows</t>
-  </si>
-  <si>
-    <t>Compost</t>
-  </si>
-  <si>
-    <t>Magic Fingers</t>
-  </si>
-  <si>
-    <t>Notched Axe</t>
-  </si>
-  <si>
-    <t>Guppys Head</t>
-  </si>
-  <si>
-    <t>Razor Blade</t>
-  </si>
-  <si>
-    <t>Wooden Nickel</t>
-  </si>
-  <si>
-    <t>Yum Heart</t>
-  </si>
-  <si>
-    <t>Portable Slot</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Monster Manual</t>
-  </si>
-  <si>
-    <t>Book of the Dead</t>
-  </si>
-  <si>
-    <t>The Necronomicon</t>
-  </si>
-  <si>
-    <t>Mega Bean</t>
-  </si>
-  <si>
-    <t>The Book of Sin</t>
-  </si>
-  <si>
-    <t>The D6</t>
-  </si>
-  <si>
-    <t>How to Jump</t>
-  </si>
-  <si>
-    <t>Unicorn Stump</t>
-  </si>
-  <si>
-    <t>The Jar</t>
-  </si>
-  <si>
-    <t>Sharp Straw</t>
-  </si>
-  <si>
-    <t>Box of Friends</t>
-  </si>
-  <si>
-    <t>Ventricle Razor</t>
-  </si>
-  <si>
-    <t>Forget Me Now</t>
-  </si>
-  <si>
-    <t>A Pony</t>
-  </si>
-  <si>
-    <t>Moms Box</t>
-  </si>
-  <si>
-    <t>Black Hole</t>
-  </si>
-  <si>
-    <t>Sacrificial Altar</t>
-  </si>
-  <si>
-    <t>The Hourglass</t>
-  </si>
-  <si>
-    <t>Teleport</t>
-  </si>
-  <si>
-    <t>Mystery Gift</t>
-  </si>
-  <si>
-    <t>Kamikaze!</t>
   </si>
 </sst>
 </file>
@@ -453,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -472,7 +493,63 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>14831</v>
+        <v>27511</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>27377</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0">
+        <v>14844</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0">
+        <v>20401</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0">
+        <v>26660</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0">
+        <v>25803</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0">
+        <v>24782</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0">
+        <v>22959</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +559,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -490,18 +567,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0">
+        <v>89522</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>119447</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0">
+        <v>59432</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>14844</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0">
+        <v>44425</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0">
+        <v>29814</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0">
+        <v>74630</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
-        <v>14831</v>
+      <c r="B9" s="0">
+        <v>104517</v>
       </c>
     </row>
   </sheetData>
@@ -519,18 +652,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0">
-        <v>14831</v>
+        <v>190337</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +673,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -551,15 +684,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0">
+        <v>72124</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>97104</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0">
+        <v>24812</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>11064</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0">
+        <v>37091</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0">
+        <v>50219</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0">
+        <v>62061</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
-        <v>11054</v>
+      <c r="B9" s="0">
+        <v>88284</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +758,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -580,15 +769,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.08668468680220943</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.08662349224082254</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0.08649650781805673</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0.08650916012781974</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0.0865764087970035</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0.08670625856555504</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
-        <v>0.08668104293275829</v>
+      <c r="B8" s="0">
+        <v>0.08670467435659462</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0.0867991990846682</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +843,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,39 +851,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0">
-        <v>1817</v>
+        <v>95</v>
       </c>
       <c r="C2" s="0">
-        <v>1817</v>
+        <v>95</v>
       </c>
       <c r="D2" s="0">
-        <v>796</v>
+        <v>72</v>
       </c>
       <c r="E2" s="0">
-        <v>7960</v>
+        <v>720</v>
       </c>
       <c r="F2" s="0">
         <v>0</v>
@@ -646,19 +891,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D3" s="0">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="F3" s="0">
         <v>0</v>
@@ -666,19 +911,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0">
-        <v>7</v>
+        <v>1213</v>
       </c>
       <c r="C4" s="0">
-        <v>7</v>
+        <v>1213</v>
       </c>
       <c r="D4" s="0">
-        <v>7</v>
+        <v>1093</v>
       </c>
       <c r="E4" s="0">
-        <v>70</v>
+        <v>10930</v>
       </c>
       <c r="F4" s="0">
         <v>0</v>
@@ -686,7 +931,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
@@ -706,19 +951,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0">
-        <v>3</v>
+        <v>220851</v>
       </c>
       <c r="C6" s="0">
-        <v>3</v>
+        <v>220851</v>
       </c>
       <c r="D6" s="0">
-        <v>3</v>
+        <v>150164</v>
       </c>
       <c r="E6" s="0">
-        <v>30</v>
+        <v>1501640</v>
       </c>
       <c r="F6" s="0">
         <v>0</v>
@@ -726,19 +971,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0">
-        <v>45</v>
+        <v>4542</v>
       </c>
       <c r="C7" s="0">
-        <v>45</v>
+        <v>4542</v>
       </c>
       <c r="D7" s="0">
-        <v>14</v>
+        <v>2263</v>
       </c>
       <c r="E7" s="0">
-        <v>140</v>
+        <v>22630</v>
       </c>
       <c r="F7" s="0">
         <v>0</v>
@@ -746,19 +991,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0">
-        <v>11974</v>
+        <v>60766</v>
       </c>
       <c r="C8" s="0">
-        <v>11974</v>
+        <v>60766</v>
       </c>
       <c r="D8" s="0">
-        <v>8139</v>
+        <v>33938</v>
       </c>
       <c r="E8" s="0">
-        <v>81390</v>
+        <v>339380</v>
       </c>
       <c r="F8" s="0">
         <v>0</v>
@@ -766,19 +1011,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0">
-        <v>204</v>
+        <v>116427</v>
       </c>
       <c r="C9" s="0">
-        <v>204</v>
+        <v>116427</v>
       </c>
       <c r="D9" s="0">
-        <v>119</v>
+        <v>49044</v>
       </c>
       <c r="E9" s="0">
-        <v>1190</v>
+        <v>490440</v>
       </c>
       <c r="F9" s="0">
         <v>0</v>
@@ -786,19 +1031,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0">
-        <v>577</v>
+        <v>3</v>
       </c>
       <c r="C10" s="0">
-        <v>577</v>
+        <v>3</v>
       </c>
       <c r="D10" s="0">
-        <v>322</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0">
-        <v>3220</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0">
         <v>0</v>
@@ -806,19 +1051,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0">
-        <v>9137</v>
+        <v>41397</v>
       </c>
       <c r="C11" s="0">
-        <v>9137</v>
+        <v>41397</v>
       </c>
       <c r="D11" s="0">
-        <v>2127</v>
+        <v>23219</v>
       </c>
       <c r="E11" s="0">
-        <v>21270</v>
+        <v>232190</v>
       </c>
       <c r="F11" s="0">
         <v>0</v>
@@ -826,21 +1071,281 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
+        <v>9</v>
+      </c>
+      <c r="B12" s="0">
+        <v>5817</v>
+      </c>
+      <c r="C12" s="0">
+        <v>5817</v>
+      </c>
+      <c r="D12" s="0">
+        <v>5112</v>
+      </c>
+      <c r="E12" s="0">
+        <v>51120</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0">
+        <v>196</v>
+      </c>
+      <c r="C13" s="0">
+        <v>196</v>
+      </c>
+      <c r="D13" s="0">
+        <v>180</v>
+      </c>
+      <c r="E13" s="0">
+        <v>1800</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0">
+        <v>2492</v>
+      </c>
+      <c r="C14" s="0">
+        <v>2492</v>
+      </c>
+      <c r="D14" s="0">
+        <v>1463</v>
+      </c>
+      <c r="E14" s="0">
+        <v>14630</v>
+      </c>
+      <c r="F14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>22</v>
+      </c>
+      <c r="B15" s="0">
+        <v>10</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0">
+        <v>20</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0">
+        <v>334090</v>
+      </c>
+      <c r="C16" s="0">
+        <v>334090</v>
+      </c>
+      <c r="D16" s="0">
+        <v>76600</v>
+      </c>
+      <c r="E16" s="0">
+        <v>766000</v>
+      </c>
+      <c r="F16" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
         <v>6</v>
       </c>
-      <c r="B12" s="0">
-        <v>69</v>
-      </c>
-      <c r="C12" s="0">
-        <v>69</v>
-      </c>
-      <c r="D12" s="0">
-        <v>57</v>
-      </c>
-      <c r="E12" s="0">
-        <v>570</v>
-      </c>
-      <c r="F12" s="0">
+      <c r="B17" s="0">
+        <v>23305</v>
+      </c>
+      <c r="C17" s="0">
+        <v>23305</v>
+      </c>
+      <c r="D17" s="0">
+        <v>17176</v>
+      </c>
+      <c r="E17" s="0">
+        <v>171760</v>
+      </c>
+      <c r="F17" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>21</v>
+      </c>
+      <c r="B18" s="0">
+        <v>7</v>
+      </c>
+      <c r="C18" s="0">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0">
+        <v>70</v>
+      </c>
+      <c r="F18" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>7</v>
+      </c>
+      <c r="B19" s="0">
+        <v>29860</v>
+      </c>
+      <c r="C19" s="0">
+        <v>29860</v>
+      </c>
+      <c r="D19" s="0">
+        <v>8901</v>
+      </c>
+      <c r="E19" s="0">
+        <v>89010</v>
+      </c>
+      <c r="F19" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>10</v>
+      </c>
+      <c r="B20" s="0">
+        <v>4977</v>
+      </c>
+      <c r="C20" s="0">
+        <v>4977</v>
+      </c>
+      <c r="D20" s="0">
+        <v>3681</v>
+      </c>
+      <c r="E20" s="0">
+        <v>36810</v>
+      </c>
+      <c r="F20" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0">
+        <v>26</v>
+      </c>
+      <c r="C21" s="0">
+        <v>26</v>
+      </c>
+      <c r="D21" s="0">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0">
+        <v>120</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>15</v>
+      </c>
+      <c r="B22" s="0">
+        <v>1386</v>
+      </c>
+      <c r="C22" s="0">
+        <v>1386</v>
+      </c>
+      <c r="D22" s="0">
+        <v>271</v>
+      </c>
+      <c r="E22" s="0">
+        <v>2710</v>
+      </c>
+      <c r="F22" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>8</v>
+      </c>
+      <c r="B23" s="0">
+        <v>7927</v>
+      </c>
+      <c r="C23" s="0">
+        <v>7927</v>
+      </c>
+      <c r="D23" s="0">
+        <v>6747</v>
+      </c>
+      <c r="E23" s="0">
+        <v>67470</v>
+      </c>
+      <c r="F23" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>17</v>
+      </c>
+      <c r="B24" s="0">
+        <v>205</v>
+      </c>
+      <c r="C24" s="0">
+        <v>205</v>
+      </c>
+      <c r="D24" s="0">
+        <v>107</v>
+      </c>
+      <c r="E24" s="0">
+        <v>1070</v>
+      </c>
+      <c r="F24" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>14</v>
+      </c>
+      <c r="B25" s="0">
+        <v>1249</v>
+      </c>
+      <c r="C25" s="0">
+        <v>1249</v>
+      </c>
+      <c r="D25" s="0">
+        <v>678</v>
+      </c>
+      <c r="E25" s="0">
+        <v>6780</v>
+      </c>
+      <c r="F25" s="0">
         <v>0</v>
       </c>
     </row>
@@ -859,27 +1364,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0">
-        <v>13</v>
+        <v>431</v>
       </c>
       <c r="C2" s="0">
-        <v>6110</v>
+        <v>163780</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -887,13 +1392,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0">
-        <v>34</v>
+        <v>427</v>
       </c>
       <c r="C3" s="0">
-        <v>340</v>
+        <v>200690</v>
       </c>
       <c r="D3" s="0">
         <v>0</v>
@@ -901,13 +1406,13 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0">
-        <v>23</v>
+        <v>421</v>
       </c>
       <c r="C4" s="0">
-        <v>2990</v>
+        <v>277860</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -915,13 +1420,13 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0">
-        <v>16</v>
+        <v>447</v>
       </c>
       <c r="C5" s="0">
-        <v>1920</v>
+        <v>312900</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -929,13 +1434,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0">
-        <v>9</v>
+        <v>436</v>
       </c>
       <c r="C6" s="0">
-        <v>5220</v>
+        <v>248520</v>
       </c>
       <c r="D6" s="0">
         <v>0</v>
@@ -943,13 +1448,13 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0">
-        <v>14</v>
+        <v>577</v>
       </c>
       <c r="C7" s="0">
-        <v>4760</v>
+        <v>98090</v>
       </c>
       <c r="D7" s="0">
         <v>0</v>
@@ -957,13 +1462,13 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0">
-        <v>15</v>
+        <v>497</v>
       </c>
       <c r="C8" s="0">
-        <v>300</v>
+        <v>144130</v>
       </c>
       <c r="D8" s="0">
         <v>0</v>
@@ -971,13 +1476,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0">
-        <v>12</v>
+        <v>551</v>
       </c>
       <c r="C9" s="0">
-        <v>8160</v>
+        <v>104690</v>
       </c>
       <c r="D9" s="0">
         <v>0</v>
@@ -985,13 +1490,13 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0">
-        <v>11</v>
+        <v>477</v>
       </c>
       <c r="C10" s="0">
-        <v>5940</v>
+        <v>310050</v>
       </c>
       <c r="D10" s="0">
         <v>0</v>
@@ -999,13 +1504,13 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0">
-        <v>18</v>
+        <v>465</v>
       </c>
       <c r="C11" s="0">
-        <v>2880</v>
+        <v>204600</v>
       </c>
       <c r="D11" s="0">
         <v>0</v>
@@ -1013,13 +1518,13 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0">
-        <v>18</v>
+        <v>444</v>
       </c>
       <c r="C12" s="0">
-        <v>540</v>
+        <v>253080</v>
       </c>
       <c r="D12" s="0">
         <v>0</v>
@@ -1027,13 +1532,13 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0">
-        <v>21</v>
+        <v>443</v>
       </c>
       <c r="C13" s="0">
-        <v>9660</v>
+        <v>261370</v>
       </c>
       <c r="D13" s="0">
         <v>0</v>
@@ -1041,13 +1546,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0">
-        <v>10</v>
+        <v>468</v>
       </c>
       <c r="C14" s="0">
-        <v>6600</v>
+        <v>159120</v>
       </c>
       <c r="D14" s="0">
         <v>0</v>
@@ -1055,13 +1560,13 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0">
-        <v>9</v>
+        <v>460</v>
       </c>
       <c r="C15" s="0">
-        <v>3420</v>
+        <v>197800</v>
       </c>
       <c r="D15" s="0">
         <v>0</v>
@@ -1069,13 +1574,13 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="C16" s="0">
-        <v>3990</v>
+        <v>254620</v>
       </c>
       <c r="D16" s="0">
         <v>0</v>
@@ -1083,13 +1588,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0">
-        <v>14</v>
+        <v>438</v>
       </c>
       <c r="C17" s="0">
-        <v>9800</v>
+        <v>157680</v>
       </c>
       <c r="D17" s="0">
         <v>0</v>
@@ -1097,13 +1602,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0">
-        <v>11</v>
+        <v>627</v>
       </c>
       <c r="C18" s="0">
-        <v>5940</v>
+        <v>62700</v>
       </c>
       <c r="D18" s="0">
         <v>0</v>
@@ -1111,13 +1616,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B19" s="0">
-        <v>23</v>
+        <v>438</v>
       </c>
       <c r="C19" s="0">
-        <v>1380</v>
+        <v>223380</v>
       </c>
       <c r="D19" s="0">
         <v>0</v>
@@ -1125,13 +1630,13 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B20" s="0">
-        <v>13</v>
+        <v>475</v>
       </c>
       <c r="C20" s="0">
-        <v>6500</v>
+        <v>237500</v>
       </c>
       <c r="D20" s="0">
         <v>0</v>
@@ -1139,13 +1644,13 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0">
-        <v>15</v>
+        <v>465</v>
       </c>
       <c r="C21" s="0">
-        <v>1950</v>
+        <v>199950</v>
       </c>
       <c r="D21" s="0">
         <v>0</v>
@@ -1153,13 +1658,13 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B22" s="0">
-        <v>13</v>
+        <v>564</v>
       </c>
       <c r="C22" s="0">
-        <v>1950</v>
+        <v>135360</v>
       </c>
       <c r="D22" s="0">
         <v>0</v>
@@ -1167,13 +1672,13 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B23" s="0">
-        <v>14</v>
+        <v>442</v>
       </c>
       <c r="C23" s="0">
-        <v>7700</v>
+        <v>238680</v>
       </c>
       <c r="D23" s="0">
         <v>0</v>
@@ -1181,13 +1686,13 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B24" s="0">
-        <v>12</v>
+        <v>463</v>
       </c>
       <c r="C24" s="0">
-        <v>2040</v>
+        <v>217610</v>
       </c>
       <c r="D24" s="0">
         <v>0</v>
@@ -1195,13 +1700,13 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B25" s="0">
-        <v>15</v>
+        <v>808</v>
       </c>
       <c r="C25" s="0">
-        <v>2400</v>
+        <v>72720</v>
       </c>
       <c r="D25" s="0">
         <v>0</v>
@@ -1209,13 +1714,13 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B26" s="0">
-        <v>26</v>
+        <v>413</v>
       </c>
       <c r="C26" s="0">
-        <v>1040</v>
+        <v>289100</v>
       </c>
       <c r="D26" s="0">
         <v>0</v>
@@ -1223,13 +1728,13 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B27" s="0">
-        <v>15</v>
+        <v>535</v>
       </c>
       <c r="C27" s="0">
-        <v>2400</v>
+        <v>90950</v>
       </c>
       <c r="D27" s="0">
         <v>0</v>
@@ -1237,13 +1742,13 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B28" s="0">
-        <v>12</v>
+        <v>493</v>
       </c>
       <c r="C28" s="0">
-        <v>2880</v>
+        <v>133110</v>
       </c>
       <c r="D28" s="0">
         <v>0</v>
@@ -1251,13 +1756,13 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B29" s="0">
-        <v>11</v>
+        <v>466</v>
       </c>
       <c r="C29" s="0">
-        <v>7700</v>
+        <v>191060</v>
       </c>
       <c r="D29" s="0">
         <v>0</v>
@@ -1265,13 +1770,13 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B30" s="0">
-        <v>15</v>
+        <v>489</v>
       </c>
       <c r="C30" s="0">
-        <v>9300</v>
+        <v>220050</v>
       </c>
       <c r="D30" s="0">
         <v>0</v>
@@ -1279,13 +1784,13 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B31" s="0">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="C31" s="0">
-        <v>150</v>
+        <v>78000</v>
       </c>
       <c r="D31" s="0">
         <v>0</v>
@@ -1293,13 +1798,13 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B32" s="0">
-        <v>20</v>
+        <v>403</v>
       </c>
       <c r="C32" s="0">
-        <v>200</v>
+        <v>274040</v>
       </c>
       <c r="D32" s="0">
         <v>0</v>
@@ -1307,13 +1812,13 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B33" s="0">
-        <v>10</v>
+        <v>435</v>
       </c>
       <c r="C33" s="0">
-        <v>900</v>
+        <v>160950</v>
       </c>
       <c r="D33" s="0">
         <v>0</v>
@@ -1321,13 +1826,13 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B34" s="0">
-        <v>16</v>
+        <v>424</v>
       </c>
       <c r="C34" s="0">
-        <v>2400</v>
+        <v>254400</v>
       </c>
       <c r="D34" s="0">
         <v>0</v>
@@ -1335,13 +1840,13 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B35" s="0">
-        <v>15</v>
+        <v>1314</v>
       </c>
       <c r="C35" s="0">
-        <v>7050</v>
+        <v>78840</v>
       </c>
       <c r="D35" s="0">
         <v>0</v>
@@ -1349,13 +1854,13 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0">
-        <v>17</v>
+        <v>435</v>
       </c>
       <c r="C36" s="0">
-        <v>11560</v>
+        <v>295800</v>
       </c>
       <c r="D36" s="0">
         <v>0</v>
@@ -1363,13 +1868,13 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B37" s="0">
-        <v>12</v>
+        <v>482</v>
       </c>
       <c r="C37" s="0">
-        <v>6600</v>
+        <v>168700</v>
       </c>
       <c r="D37" s="0">
         <v>0</v>
@@ -1377,13 +1882,13 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B38" s="0">
-        <v>16</v>
+        <v>455</v>
       </c>
       <c r="C38" s="0">
-        <v>6720</v>
+        <v>182000</v>
       </c>
       <c r="D38" s="0">
         <v>0</v>
@@ -1391,13 +1896,13 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0">
-        <v>8</v>
+        <v>521</v>
       </c>
       <c r="C39" s="0">
-        <v>4880</v>
+        <v>140670</v>
       </c>
       <c r="D39" s="0">
         <v>0</v>
@@ -1405,13 +1910,13 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B40" s="0">
-        <v>15</v>
+        <v>738</v>
       </c>
       <c r="C40" s="0">
-        <v>9900</v>
+        <v>14760</v>
       </c>
       <c r="D40" s="0">
         <v>0</v>
@@ -1419,13 +1924,13 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B41" s="0">
-        <v>10</v>
+        <v>2005</v>
       </c>
       <c r="C41" s="0">
-        <v>3400</v>
+        <v>60150</v>
       </c>
       <c r="D41" s="0">
         <v>0</v>
@@ -1433,13 +1938,13 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B42" s="0">
-        <v>13</v>
+        <v>652</v>
       </c>
       <c r="C42" s="0">
-        <v>5070</v>
+        <v>71720</v>
       </c>
       <c r="D42" s="0">
         <v>0</v>
@@ -1447,13 +1952,13 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B43" s="0">
-        <v>13</v>
+        <v>443</v>
       </c>
       <c r="C43" s="0">
-        <v>5200</v>
+        <v>239220</v>
       </c>
       <c r="D43" s="0">
         <v>0</v>
@@ -1461,13 +1966,13 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B44" s="0">
-        <v>11</v>
+        <v>399</v>
       </c>
       <c r="C44" s="0">
-        <v>3300</v>
+        <v>159600</v>
       </c>
       <c r="D44" s="0">
         <v>0</v>
@@ -1475,13 +1980,13 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B45" s="0">
-        <v>19</v>
+        <v>533</v>
       </c>
       <c r="C45" s="0">
-        <v>1140</v>
+        <v>85280</v>
       </c>
       <c r="D45" s="0">
         <v>0</v>
@@ -1489,13 +1994,13 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B46" s="0">
-        <v>14</v>
+        <v>449</v>
       </c>
       <c r="C46" s="0">
-        <v>6160</v>
+        <v>170620</v>
       </c>
       <c r="D46" s="0">
         <v>0</v>
@@ -1503,13 +2008,13 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B47" s="0">
-        <v>7</v>
+        <v>447</v>
       </c>
       <c r="C47" s="0">
-        <v>3150</v>
+        <v>192210</v>
       </c>
       <c r="D47" s="0">
         <v>0</v>
@@ -1517,13 +2022,13 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B48" s="0">
-        <v>8</v>
+        <v>548</v>
       </c>
       <c r="C48" s="0">
-        <v>1520</v>
+        <v>87680</v>
       </c>
       <c r="D48" s="0">
         <v>0</v>
@@ -1531,13 +2036,13 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B49" s="0">
-        <v>19</v>
+        <v>413</v>
       </c>
       <c r="C49" s="0">
-        <v>3230</v>
+        <v>227150</v>
       </c>
       <c r="D49" s="0">
         <v>0</v>
@@ -1545,13 +2050,13 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B50" s="0">
-        <v>13</v>
+        <v>422</v>
       </c>
       <c r="C50" s="0">
-        <v>5330</v>
+        <v>215220</v>
       </c>
       <c r="D50" s="0">
         <v>0</v>
@@ -1559,13 +2064,13 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B51" s="0">
-        <v>13</v>
+        <v>561</v>
       </c>
       <c r="C51" s="0">
-        <v>6890</v>
+        <v>89760</v>
       </c>
       <c r="D51" s="0">
         <v>0</v>
@@ -1573,13 +2078,13 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B52" s="0">
-        <v>14</v>
+        <v>474</v>
       </c>
       <c r="C52" s="0">
-        <v>6020</v>
+        <v>165900</v>
       </c>
       <c r="D52" s="0">
         <v>0</v>
@@ -1587,13 +2092,13 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B53" s="0">
-        <v>7</v>
+        <v>458</v>
       </c>
       <c r="C53" s="0">
-        <v>4060</v>
+        <v>146560</v>
       </c>
       <c r="D53" s="0">
         <v>0</v>
@@ -1601,13 +2106,13 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B54" s="0">
-        <v>16</v>
+        <v>1985</v>
       </c>
       <c r="C54" s="0">
-        <v>1600</v>
+        <v>19850</v>
       </c>
       <c r="D54" s="0">
         <v>0</v>
@@ -1615,13 +2120,13 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B55" s="0">
-        <v>16</v>
+        <v>448</v>
       </c>
       <c r="C55" s="0">
-        <v>10400</v>
+        <v>304640</v>
       </c>
       <c r="D55" s="0">
         <v>0</v>
@@ -1629,13 +2134,13 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B56" s="0">
-        <v>10</v>
+        <v>2084</v>
       </c>
       <c r="C56" s="0">
-        <v>100</v>
+        <v>20840</v>
       </c>
       <c r="D56" s="0">
         <v>0</v>
@@ -1643,13 +2148,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B57" s="0">
-        <v>10</v>
+        <v>438</v>
       </c>
       <c r="C57" s="0">
-        <v>2700</v>
+        <v>201480</v>
       </c>
       <c r="D57" s="0">
         <v>0</v>
@@ -1657,13 +2162,13 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B58" s="0">
-        <v>9</v>
+        <v>1976</v>
       </c>
       <c r="C58" s="0">
-        <v>5850</v>
+        <v>19760</v>
       </c>
       <c r="D58" s="0">
         <v>0</v>
@@ -1671,13 +2176,13 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B59" s="0">
-        <v>9</v>
+        <v>474</v>
       </c>
       <c r="C59" s="0">
-        <v>3150</v>
+        <v>184860</v>
       </c>
       <c r="D59" s="0">
         <v>0</v>
@@ -1685,13 +2190,13 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B60" s="0">
-        <v>15</v>
+        <v>419</v>
       </c>
       <c r="C60" s="0">
-        <v>7500</v>
+        <v>293300</v>
       </c>
       <c r="D60" s="0">
         <v>0</v>
@@ -1699,13 +2204,13 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B61" s="0">
-        <v>14</v>
+        <v>2024</v>
       </c>
       <c r="C61" s="0">
-        <v>3780</v>
+        <v>20240</v>
       </c>
       <c r="D61" s="0">
         <v>0</v>
@@ -1713,13 +2218,13 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B62" s="0">
-        <v>11</v>
+        <v>562</v>
       </c>
       <c r="C62" s="0">
-        <v>3960</v>
+        <v>73060</v>
       </c>
       <c r="D62" s="0">
         <v>0</v>
@@ -1727,13 +2232,13 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B63" s="0">
-        <v>20</v>
+        <v>436</v>
       </c>
       <c r="C63" s="0">
-        <v>4800</v>
+        <v>244160</v>
       </c>
       <c r="D63" s="0">
         <v>0</v>
@@ -1741,13 +2246,13 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B64" s="0">
-        <v>19</v>
+        <v>2045</v>
       </c>
       <c r="C64" s="0">
-        <v>10260</v>
+        <v>40900</v>
       </c>
       <c r="D64" s="0">
         <v>0</v>
@@ -1755,13 +2260,13 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B65" s="0">
-        <v>9</v>
+        <v>556</v>
       </c>
       <c r="C65" s="0">
-        <v>3420</v>
+        <v>133440</v>
       </c>
       <c r="D65" s="0">
         <v>0</v>
@@ -1769,13 +2274,13 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B66" s="0">
-        <v>16</v>
+        <v>435</v>
       </c>
       <c r="C66" s="0">
-        <v>5440</v>
+        <v>269700</v>
       </c>
       <c r="D66" s="0">
         <v>0</v>
@@ -1783,13 +2288,13 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B67" s="0">
-        <v>16</v>
+        <v>744</v>
       </c>
       <c r="C67" s="0">
-        <v>9120</v>
+        <v>74400</v>
       </c>
       <c r="D67" s="0">
         <v>0</v>
@@ -1797,13 +2302,13 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B68" s="0">
-        <v>11</v>
+        <v>423</v>
       </c>
       <c r="C68" s="0">
-        <v>1100</v>
+        <v>253800</v>
       </c>
       <c r="D68" s="0">
         <v>0</v>
@@ -1811,13 +2316,13 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B69" s="0">
-        <v>15</v>
+        <v>484</v>
       </c>
       <c r="C69" s="0">
-        <v>1050</v>
+        <v>203280</v>
       </c>
       <c r="D69" s="0">
         <v>0</v>
@@ -1825,13 +2330,13 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B70" s="0">
-        <v>16</v>
+        <v>1916</v>
       </c>
       <c r="C70" s="0">
-        <v>4320</v>
+        <v>76640</v>
       </c>
       <c r="D70" s="0">
         <v>0</v>
@@ -1839,13 +2344,13 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B71" s="0">
-        <v>16</v>
+        <v>1974</v>
       </c>
       <c r="C71" s="0">
-        <v>5760</v>
+        <v>19740</v>
       </c>
       <c r="D71" s="0">
         <v>0</v>
@@ -1853,13 +2358,13 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B72" s="0">
-        <v>10</v>
+        <v>526</v>
       </c>
       <c r="C72" s="0">
-        <v>2700</v>
+        <v>89420</v>
       </c>
       <c r="D72" s="0">
         <v>0</v>
@@ -1867,13 +2372,13 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B73" s="0">
-        <v>10</v>
+        <v>410</v>
       </c>
       <c r="C73" s="0">
-        <v>4000</v>
+        <v>258300</v>
       </c>
       <c r="D73" s="0">
         <v>0</v>
@@ -1881,13 +2386,13 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B74" s="0">
-        <v>17</v>
+        <v>471</v>
       </c>
       <c r="C74" s="0">
-        <v>1700</v>
+        <v>160140</v>
       </c>
       <c r="D74" s="0">
         <v>0</v>
@@ -1895,13 +2400,13 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B75" s="0">
-        <v>11</v>
+        <v>479</v>
       </c>
       <c r="C75" s="0">
-        <v>3300</v>
+        <v>249080</v>
       </c>
       <c r="D75" s="0">
         <v>0</v>
@@ -1909,13 +2414,13 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B76" s="0">
-        <v>12</v>
+        <v>1084</v>
       </c>
       <c r="C76" s="0">
-        <v>3960</v>
+        <v>75880</v>
       </c>
       <c r="D76" s="0">
         <v>0</v>
@@ -1923,13 +2428,13 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B77" s="0">
-        <v>17</v>
+        <v>469</v>
       </c>
       <c r="C77" s="0">
-        <v>7310</v>
+        <v>253260</v>
       </c>
       <c r="D77" s="0">
         <v>0</v>
@@ -1937,13 +2442,13 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B78" s="0">
-        <v>14</v>
+        <v>470</v>
       </c>
       <c r="C78" s="0">
-        <v>9520</v>
+        <v>169200</v>
       </c>
       <c r="D78" s="0">
         <v>0</v>
@@ -1951,13 +2456,13 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B79" s="0">
-        <v>12</v>
+        <v>433</v>
       </c>
       <c r="C79" s="0">
-        <v>7560</v>
+        <v>216500</v>
       </c>
       <c r="D79" s="0">
         <v>0</v>
@@ -1965,13 +2470,13 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B80" s="0">
-        <v>19</v>
+        <v>469</v>
       </c>
       <c r="C80" s="0">
-        <v>9310</v>
+        <v>140700</v>
       </c>
       <c r="D80" s="0">
         <v>0</v>
@@ -1979,13 +2484,13 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B81" s="0">
-        <v>9</v>
+        <v>426</v>
       </c>
       <c r="C81" s="0">
-        <v>5040</v>
+        <v>208740</v>
       </c>
       <c r="D81" s="0">
         <v>0</v>
@@ -1993,13 +2498,13 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B82" s="0">
-        <v>11</v>
+        <v>446</v>
       </c>
       <c r="C82" s="0">
-        <v>7480</v>
+        <v>223000</v>
       </c>
       <c r="D82" s="0">
         <v>0</v>
@@ -2007,13 +2512,13 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B83" s="0">
-        <v>12</v>
+        <v>445</v>
       </c>
       <c r="C83" s="0">
-        <v>3480</v>
+        <v>244750</v>
       </c>
       <c r="D83" s="0">
         <v>0</v>
@@ -2021,13 +2526,13 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B84" s="0">
-        <v>13</v>
+        <v>808</v>
       </c>
       <c r="C84" s="0">
-        <v>6500</v>
+        <v>72720</v>
       </c>
       <c r="D84" s="0">
         <v>0</v>
@@ -2035,13 +2540,13 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B85" s="0">
-        <v>16</v>
+        <v>587</v>
       </c>
       <c r="C85" s="0">
-        <v>10080</v>
+        <v>88050</v>
       </c>
       <c r="D85" s="0">
         <v>0</v>
@@ -2049,13 +2554,13 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B86" s="0">
-        <v>17</v>
+        <v>597</v>
       </c>
       <c r="C86" s="0">
-        <v>8670</v>
+        <v>95520</v>
       </c>
       <c r="D86" s="0">
         <v>0</v>
@@ -2063,13 +2568,13 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B87" s="0">
-        <v>10</v>
+        <v>444</v>
       </c>
       <c r="C87" s="0">
-        <v>2200</v>
+        <v>150960</v>
       </c>
       <c r="D87" s="0">
         <v>0</v>
@@ -2077,13 +2582,13 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B88" s="0">
-        <v>9</v>
+        <v>459</v>
       </c>
       <c r="C88" s="0">
-        <v>5310</v>
+        <v>312120</v>
       </c>
       <c r="D88" s="0">
         <v>0</v>
@@ -2091,13 +2596,13 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B89" s="0">
-        <v>21</v>
+        <v>420</v>
       </c>
       <c r="C89" s="0">
-        <v>3570</v>
+        <v>189000</v>
       </c>
       <c r="D89" s="0">
         <v>0</v>
@@ -2105,13 +2610,13 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B90" s="0">
-        <v>11</v>
+        <v>433</v>
       </c>
       <c r="C90" s="0">
-        <v>1210</v>
+        <v>272790</v>
       </c>
       <c r="D90" s="0">
         <v>0</v>
@@ -2119,13 +2624,13 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B91" s="0">
-        <v>6</v>
+        <v>444</v>
       </c>
       <c r="C91" s="0">
-        <v>2100</v>
+        <v>288600</v>
       </c>
       <c r="D91" s="0">
         <v>0</v>
@@ -2133,13 +2638,13 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B92" s="0">
-        <v>10</v>
+        <v>424</v>
       </c>
       <c r="C92" s="0">
-        <v>4100</v>
+        <v>173840</v>
       </c>
       <c r="D92" s="0">
         <v>0</v>
@@ -2147,13 +2652,13 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B93" s="0">
-        <v>11</v>
+        <v>434</v>
       </c>
       <c r="C93" s="0">
-        <v>3740</v>
+        <v>251720</v>
       </c>
       <c r="D93" s="0">
         <v>0</v>
@@ -2161,13 +2666,13 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B94" s="0">
-        <v>7</v>
+        <v>484</v>
       </c>
       <c r="C94" s="0">
-        <v>3010</v>
+        <v>130680</v>
       </c>
       <c r="D94" s="0">
         <v>0</v>
@@ -2175,13 +2680,13 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B95" s="0">
-        <v>22</v>
+        <v>496</v>
       </c>
       <c r="C95" s="0">
-        <v>440</v>
+        <v>143840</v>
       </c>
       <c r="D95" s="0">
         <v>0</v>
@@ -2189,13 +2694,13 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B96" s="0">
-        <v>11</v>
+        <v>493</v>
       </c>
       <c r="C96" s="0">
-        <v>4950</v>
+        <v>192270</v>
       </c>
       <c r="D96" s="0">
         <v>0</v>
@@ -2203,13 +2708,13 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B97" s="0">
-        <v>12</v>
+        <v>448</v>
       </c>
       <c r="C97" s="0">
-        <v>6240</v>
+        <v>295680</v>
       </c>
       <c r="D97" s="0">
         <v>0</v>
@@ -2217,13 +2722,13 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B98" s="0">
-        <v>14</v>
+        <v>461</v>
       </c>
       <c r="C98" s="0">
-        <v>1260</v>
+        <v>235110</v>
       </c>
       <c r="D98" s="0">
         <v>0</v>
@@ -2231,13 +2736,13 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B99" s="0">
-        <v>10</v>
+        <v>924</v>
       </c>
       <c r="C99" s="0">
-        <v>3900</v>
+        <v>73920</v>
       </c>
       <c r="D99" s="0">
         <v>0</v>
@@ -2245,13 +2750,13 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B100" s="0">
-        <v>16</v>
+        <v>525</v>
       </c>
       <c r="C100" s="0">
-        <v>10560</v>
+        <v>115500</v>
       </c>
       <c r="D100" s="0">
         <v>0</v>
@@ -2259,13 +2764,13 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B101" s="0">
-        <v>15</v>
+        <v>578</v>
       </c>
       <c r="C101" s="0">
-        <v>9000</v>
+        <v>86700</v>
       </c>
       <c r="D101" s="0">
         <v>0</v>
@@ -2273,13 +2778,13 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B102" s="0">
-        <v>15</v>
+        <v>675</v>
       </c>
       <c r="C102" s="0">
-        <v>7650</v>
+        <v>74250</v>
       </c>
       <c r="D102" s="0">
         <v>0</v>
@@ -2287,13 +2792,13 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B103" s="0">
-        <v>18</v>
+        <v>792</v>
       </c>
       <c r="C103" s="0">
-        <v>12600</v>
+        <v>79200</v>
       </c>
       <c r="D103" s="0">
         <v>0</v>
@@ -2301,13 +2806,13 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B104" s="0">
-        <v>9</v>
+        <v>531</v>
       </c>
       <c r="C104" s="0">
-        <v>990</v>
+        <v>79650</v>
       </c>
       <c r="D104" s="0">
         <v>0</v>
@@ -2315,13 +2820,13 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B105" s="0">
-        <v>11</v>
+        <v>448</v>
       </c>
       <c r="C105" s="0">
-        <v>3190</v>
+        <v>147840</v>
       </c>
       <c r="D105" s="0">
         <v>0</v>
@@ -2329,13 +2834,13 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B106" s="0">
-        <v>15</v>
+        <v>471</v>
       </c>
       <c r="C106" s="0">
-        <v>4800</v>
+        <v>141300</v>
       </c>
       <c r="D106" s="0">
         <v>0</v>
@@ -2343,13 +2848,13 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B107" s="0">
-        <v>19</v>
+        <v>559</v>
       </c>
       <c r="C107" s="0">
-        <v>3040</v>
+        <v>150930</v>
       </c>
       <c r="D107" s="0">
         <v>0</v>
@@ -2357,13 +2862,13 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B108" s="0">
-        <v>14</v>
+        <v>426</v>
       </c>
       <c r="C108" s="0">
-        <v>6580</v>
+        <v>259860</v>
       </c>
       <c r="D108" s="0">
         <v>0</v>
@@ -2371,13 +2876,13 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B109" s="0">
-        <v>11</v>
+        <v>424</v>
       </c>
       <c r="C109" s="0">
-        <v>5610</v>
+        <v>279840</v>
       </c>
       <c r="D109" s="0">
         <v>0</v>
@@ -2385,13 +2890,13 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B110" s="0">
-        <v>7</v>
+        <v>628</v>
       </c>
       <c r="C110" s="0">
-        <v>4200</v>
+        <v>75360</v>
       </c>
       <c r="D110" s="0">
         <v>0</v>
@@ -2399,13 +2904,13 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B111" s="0">
-        <v>19</v>
+        <v>507</v>
       </c>
       <c r="C111" s="0">
-        <v>1520</v>
+        <v>172380</v>
       </c>
       <c r="D111" s="0">
         <v>0</v>
@@ -2413,13 +2918,13 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B112" s="0">
-        <v>20</v>
+        <v>459</v>
       </c>
       <c r="C112" s="0">
-        <v>200</v>
+        <v>215730</v>
       </c>
       <c r="D112" s="0">
         <v>0</v>
@@ -2427,13 +2932,13 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B113" s="0">
-        <v>19</v>
+        <v>1302</v>
       </c>
       <c r="C113" s="0">
-        <v>2850</v>
+        <v>78120</v>
       </c>
       <c r="D113" s="0">
         <v>0</v>
@@ -2441,13 +2946,13 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B114" s="0">
-        <v>10</v>
+        <v>474</v>
       </c>
       <c r="C114" s="0">
-        <v>3700</v>
+        <v>251220</v>
       </c>
       <c r="D114" s="0">
         <v>0</v>

</xml_diff>